<commit_message>
correct some issues with tag ids and start curve fitting
</commit_message>
<xml_diff>
--- a/licor_data/licor_log_files/stan_log_05062023.xlsx
+++ b/licor_data/licor_log_files/stan_log_05062023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/trillium_trail/licor_data/licor_log_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E7221FE-5E94-2742-9B8D-E5133E16A737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB52A2C6-9E2E-F944-A84B-DA34A42DDD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4060" yWindow="500" windowWidth="28800" windowHeight="23260" xr2:uid="{E2101264-4A8C-BA4C-A9EF-E5EFE562CDE8}"/>
+    <workbookView xWindow="19860" yWindow="500" windowWidth="28800" windowHeight="23260" xr2:uid="{E2101264-4A8C-BA4C-A9EF-E5EFE562CDE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -243,15 +243,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,7 +572,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -689,7 +689,7 @@
     </row>
     <row r="5" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="6">
-        <v>5075</v>
+        <v>5073</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>18</v>
@@ -1104,14 +1104,14 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="39" x14ac:dyDescent="0.45">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
     </row>
     <row r="22" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
@@ -1120,61 +1120,61 @@
       <c r="B22" s="3"/>
     </row>
     <row r="23" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="9"/>
+      <c r="B23" s="12"/>
       <c r="C23" s="4">
         <v>500</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F23" s="9"/>
+      <c r="F23" s="12"/>
       <c r="G23" s="4">
         <v>10000</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="9"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="4">
         <v>1.5</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F24" s="10"/>
+      <c r="F24" s="13"/>
       <c r="G24" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="9"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="10"/>
+      <c r="F25" s="13"/>
       <c r="G25" s="4">
         <v>1600</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="26" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>